<commit_message>
feat : 환자 등록하기 기능 구현, patient_form.html 제작
</commit_message>
<xml_diff>
--- a/API 명세서.xlsx
+++ b/API 명세서.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\DBPJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC9F0E43-5575-43D2-A2A4-AC90353F8FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02899E16-D95F-487E-85C8-CC3F05DCFC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5400" yWindow="30" windowWidth="16200" windowHeight="11273" xr2:uid="{7B00C6B7-C6CC-4199-B763-6D78FF28C116}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,6 +60,30 @@
   </si>
   <si>
     <t>해당 아이디의 환자 정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환자 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환자 정보 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환자 삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -518,123 +542,147 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat : make TestRecords_api and related things
</commit_message>
<xml_diff>
--- a/API 명세서.xlsx
+++ b/API 명세서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\DBPJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B8CCFF-FBEF-4BC0-846E-9EA114B17288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49C298C-62B1-44F0-8DA1-954C29AC1431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="30" windowWidth="16200" windowHeight="11273" xr2:uid="{7B00C6B7-C6CC-4199-B763-6D78FF28C116}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{7B00C6B7-C6CC-4199-B763-6D78FF28C116}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>환자 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DELETE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -88,6 +84,26 @@
   </si>
   <si>
     <t>/api/create_patient</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api2/create_TestRecords/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api2/TestRecords/&lt;int:pk&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 코드의 검사 데이터 조회 (해당 코드는 환자와 연관 X)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검사 데이터 추가 ( 템플릿 )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환자 추가 ( 템플릿 )</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -490,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F84D3-9DDD-44BB-B172-254F222F9B43}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -499,7 +515,7 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="17.9375" customWidth="1"/>
     <col min="3" max="3" width="63.0625" customWidth="1"/>
-    <col min="4" max="4" width="40.3125" customWidth="1"/>
+    <col min="4" max="4" width="49.5625" customWidth="1"/>
     <col min="5" max="5" width="24.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -553,10 +569,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.6">
@@ -564,13 +580,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.6">
@@ -578,26 +594,42 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="2"/>
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A9" s="3"/>

</xml_diff>

<commit_message>
feat : make DiagonosticRecords_api and related forms
</commit_message>
<xml_diff>
--- a/API 명세서.xlsx
+++ b/API 명세서.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\DBPJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49C298C-62B1-44F0-8DA1-954C29AC1431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821E3921-22A0-451F-A59B-7CC7B327BD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{7B00C6B7-C6CC-4199-B763-6D78FF28C116}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -104,6 +104,14 @@
   </si>
   <si>
     <t>환자 추가 ( 템플릿 )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api3/create_diagnosis/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진료 데이터 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -507,7 +515,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -633,9 +641,15 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A10" s="3"/>

</xml_diff>

<commit_message>
feat : make Prescription_api and related forms.html
</commit_message>
<xml_diff>
--- a/API 명세서.xlsx
+++ b/API 명세서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\DBPJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821E3921-22A0-451F-A59B-7CC7B327BD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194EAE00-030A-4F1B-945A-0657F7D41BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{7B00C6B7-C6CC-4199-B763-6D78FF28C116}"/>
+    <workbookView xWindow="2348" yWindow="127" windowWidth="16199" windowHeight="11273" xr2:uid="{7B00C6B7-C6CC-4199-B763-6D78FF28C116}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -112,6 +112,14 @@
   </si>
   <si>
     <t>진료 데이터 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api4/create_prescription/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>처방 데이터 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -515,7 +523,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -640,7 +648,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A9" s="3"/>
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
@@ -652,10 +662,18 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A11" s="3"/>

</xml_diff>

<commit_message>
feat : make TreatmentRecords_api and related forms
</commit_message>
<xml_diff>
--- a/API 명세서.xlsx
+++ b/API 명세서.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\DBPJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194EAE00-030A-4F1B-945A-0657F7D41BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8DB2E8-FB3F-4CF8-95B7-B02103FD9BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2348" yWindow="127" windowWidth="16199" windowHeight="11273" xr2:uid="{7B00C6B7-C6CC-4199-B763-6D78FF28C116}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,6 +120,13 @@
   </si>
   <si>
     <t>처방 데이터 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api5/create_treatment/</t>
+  </si>
+  <si>
+    <t>치료 데이터 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -522,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F84D3-9DDD-44BB-B172-254F222F9B43}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -676,10 +683,18 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A12" s="3"/>

</xml_diff>

<commit_message>
feat : make ExerciseRecords_api and related form
</commit_message>
<xml_diff>
--- a/API 명세서.xlsx
+++ b/API 명세서.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\DBPJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8DB2E8-FB3F-4CF8-95B7-B02103FD9BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD7A46F-2435-41B6-82C8-B4FC402C3E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2348" yWindow="127" windowWidth="16199" windowHeight="11273" xr2:uid="{7B00C6B7-C6CC-4199-B763-6D78FF28C116}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,6 +127,14 @@
   </si>
   <si>
     <t>치료 데이터 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>운동 데이터 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api6/create_exercise/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -529,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F84D3-9DDD-44BB-B172-254F222F9B43}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -697,10 +705,18 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A13" s="3"/>

</xml_diff>